<commit_message>
Update Inputs and Outputs files
</commit_message>
<xml_diff>
--- a/outputs/xlsx/roles.xlsx
+++ b/outputs/xlsx/roles.xlsx
@@ -542,7 +542,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>[&lt;Member id=811574480299491338 name='Lorette CJ Saint Pierre du Mont' discriminator='1730' bot=False nick='Lorette - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=815284094417764383 name='Capucine CJ de Plaisir' discriminator='2186' bot=False nick='Capucine - Plaisir (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=573070802577129473 name="Romain CJ de Yvré l'Évèque" discriminator='9972' bot=False nick="Romain - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=821843675272970272 name='Club jeunes Chamarande' discriminator='6857' bot=False nick='Léa - Chamarande (91)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=831266666486562846 name='lilium' discriminator='2421' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=812420035493625947 name="Mathéa.s de Yvré l'éveque 72" discriminator='3239' bot=False nick="Mathéa.s - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=688137172179615745 name='🌟 「 𝔹𝕒𝕓𝕪 𝕘𝕚𝕣𝕝 」 🌟' discriminator='7001' bot=False nick="Timothé - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=569597210728071210 name='Louve' discriminator='1683' bot=False nick='Laureline - Plaisir (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=819170497132363799 name='Ereann cj vaux le penil' discriminator='2086' bot=False nick='Ereann - Vaux-le-Pénil (77)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=691588451547480076 name='Stéph_of28' discriminator='9983' bot=False nick='Stéphanie - Saint-Omer (62)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=812289741294534718 name='Noelly CJ de Chameyrat' discriminator='1221' bot=False nick='Noelly - Chameyrat (19)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=439791430651609089 name='Repti' discriminator='9965' bot=False nick='Enzo - Saint-Omer (62)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817369610051125309 name='Clémence' discriminator='9498' bot=False nick="Clémence - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=828949602937864202 name='Anne-Sophie - Forbach (57)' discriminator='7869' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=704237474221654086 name='léa' discriminator='3402' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=816646879135793152 name='titouan de poulainville' discriminator='6643' bot=False nick='Titouan - Poulainville (80)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=674885857458651161 name='MemberList' discriminator='4997' bot=True nick='🐶Hachikō' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=818559139415719976 name='KimieCJduGarric' discriminator='7403' bot=False nick='Kimie - Le Garric (81)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=231129972755005440 name='Oyoelle' discriminator='7903' bot=False nick='Elwenn - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=816751853026017361 name='Lony cj poulainville' discriminator='5437' bot=False nick='Lony - Poulainville (80)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=653187728032399391 name='ImnotnathaYT' discriminator='8079' bot=False nick='Nathael - Bordeaux (33)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=821072189080076328 name='Marine du CJ de la Roche sur Yon' discriminator='0978' bot=False nick='Marine - La Roche-sur-Yon (85)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=752240686992064693 name='Meli melo' discriminator='9181' bot=False nick='Meryam - Forbach (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=828320232971829299 name='julie37' discriminator='9767' bot=False nick='Julie - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=683034848981680129 name="lily_blk CJ de yvré l'évêque" discriminator='7445' bot=False nick="Lily - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=766218397536354335 name='Abel_j' discriminator='2508' bot=False nick='Abel - Chamarande (91)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=809820884553826415 name='magic-Tim' discriminator='2385' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=689400323713794078 name='Marie-Agnès' discriminator='5423' bot=False nick='Marie-Agnès - Orgeval (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=811897434225377280 name='Héloïse CJ de Chameyrat' discriminator='5373' bot=False nick='Héloïse - Chameyrat (19)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=689473018740998159 name='Cathy' discriminator='7851' bot=False nick='Cathy - Sarreguemines (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=689815595746590832 name='jtmfort' discriminator='1427' bot=False nick='Lola - Vaux-le-Pénil (77)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=811893356618579978 name='Lily CJ de Rennes' discriminator='3212' bot=False nick='Lily - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=812625585276846130 name='YACINE CJ PLAISIR 78' discriminator='7816' bot=False nick='Yacine - Plaisir (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=822061661564174348 name='Nils05100' discriminator='4521' bot=False nick='Nils - Briançon (05)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=333364261688442890 name='Lucas ²' discriminator='1486' bot=False nick='Lucas - Forbach (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=811688103668219915 name='Lily CJ de Rennes' discriminator='0920' bot=False nick='Lily - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=806174253849378839 name='Kévin DOUANGSAVATH' discriminator='6501' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=812780108036571136 name='Chiara CJ de Niort' discriminator='8059' bot=False nick='Chiara - Niort (79)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=666896278021472287 name='Cassou-edn' discriminator='0209' bot=False nick="Cassandre - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=774024415859834911 name='malena' discriminator='8914' bot=False nick='Maléna - Cholet (49)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=694309330429804545 name='Valentine' discriminator='5125' bot=False nick='Valentine - Saint-Omer (62)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817867946701226003 name='paupau' discriminator='2647' bot=False nick='Pauline - Forbach (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=832180379527282688 name='lilou37' discriminator='1946' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=814861125580881940 name='Léane du CJ de Plaisir' discriminator='1982' bot=False nick='Léane - Plaisir (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=324631108731928587 name='Simple Poll' discriminator='9879' bot=True nick='🐶Laïka' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=826134409349955594 name='Mary-Chateaubourg35' discriminator='3382' bot=False nick='Mary - Chateaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=812399451427307542 name='sarah kervinio Yvré' discriminator='5630' bot=False nick="Sarah - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817494596170416128 name='Dragana' discriminator='8632' bot=False nick='Dragana - Laon (02)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=791638268247801898 name='Lucie - Forbach (57)' discriminator='7764' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=777226843963129926 name='Evangéline' discriminator='9710' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817462125815398411 name='Cécile Encadrante CJ Luynes (37)' discriminator='4741' bot=False nick='Cécile - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=689063301199822971 name='Loane' discriminator='5676' bot=False nick='Loane - Chamarande (91)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=689875189814657053 name='Hélène - Encadrante SPA - Millau' discriminator='0248' bot=False nick='Hélène - Millau (12)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=410138084181671938 name='Aiglor009' discriminator='3918' bot=False nick='Thomas - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=824269174246998076 name='Louna CJ de Luynes' discriminator='1106' bot=False nick='Louna - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=812023228167618601 name='Sylvie CJ St OMER' discriminator='3410' bot=False nick='Sylvie - Saint-Omer (62)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=821332977371185152 name='catherine vitre' discriminator='6716' bot=False nick='Catherine - Vitré (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=811685909669216287 name='Lily CJ de Rennes' discriminator='7358' bot=False nick='Lily - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=820921651343785985 name='Sophie RADIDEAU ROBINE' discriminator='2033' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817630483294060595 name='Catherine Fuseau' discriminator='8144' bot=False nick='Catherine - SPAT (10)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=826888582060179516 name='Laura CJ St Pierre du Mont' discriminator='3104' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=826007429703532545 name='Cassy CJ de Chamarande' discriminator='3125' bot=False nick='Cassy - Chamarande (91)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=725471539365150867 name='Erwan' discriminator='0084' bot=False nick='Erwan - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817456802983575553 name='Alix CJ SPDM' discriminator='4012' bot=False nick='Alix - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=772050348592201729 name='maelys CJ Pornic' discriminator='7949' bot=False nick='Maelys - Pornic (44)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817472074028941322 name='Marinette CJ de Luynes' discriminator='4290' bot=False nick='Marinette - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=614958426849542157 name="Le P'tit Beurre Fou" discriminator='3503' bot=False nick='Eliott - Briançon (05)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=823644993427865690 name='Manonmr' discriminator='6723' bot=False nick='Manon - Le Garric (81)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=713390694806323312 name='Justine' discriminator='8951' bot=False nick='Justine - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=820014965867151370 name='erine du CJ de vaux le penil' discriminator='0120' bot=False nick='Erine - Vaux-le-Pénil (77)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=813532163655729172 name='Kelly CJ De Luynes' discriminator='4055' bot=False nick='Kelly - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=814843246046871604 name='Héléna CJ de Laon' discriminator='0749' bot=False nick='Héléna - Laon (02)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=723818066932269137 name='Marianne' discriminator='0263' bot=False nick='Marianne - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=814539477057011762 name='Clementine CJ de Millau' discriminator='9234' bot=False nick='Clementine - Millau (12)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817494454927491093 name='Maria CJ La Roche sur Yon' discriminator='7686' bot=False nick='Maria - La Roche-sur-Yon (85)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=689831329331675143 name='Marywenn.Pornic(44)' discriminator='1346' bot=False nick='Maryween - Pornic (44)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=765294557252157440 name='Anaël CJ de Cluses' discriminator='7963' bot=False nick='Anaël - Cluses (74)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=818083516234989588 name='Chantale CJ de Plaisir' discriminator='3278' bot=False nick='Chantale - Plaisir (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=818128336185196544 name='Lena Raimbaud' discriminator='9590' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=796103288646926437 name='Garance' discriminator='7603' bot=False nick='Garance - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=690509463924506626 name='nightfox' discriminator='9964' bot=False nick='Esteban - Plaisir (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=819282970023559180 name='ines Cj thionville' discriminator='1353' bot=False nick='Inès - Thionville (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=814469566595596288 name='Lily CJ de Rennes' discriminator='3091' bot=False nick='Lily - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=811576583613579324 name='soizic du CJ de la roche sur yon' discriminator='8969' bot=False nick='Soizic - La Roche-sur-Yon (85)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=717309388830015528 name='Héloïse CJ de Pornic' discriminator='6617' bot=False nick='Héloise - Pornic (44)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=826007033266176011 name='Cassy CJ de Chamarande' discriminator='6404' bot=False nick='Cassy - Chamarande (91)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=825621468679110656 name='Lola du CJ du Garric' discriminator='6051' bot=False nick='Lola - Le Garric (81)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=793473737310601227 name='Alicia CJ de Menois' discriminator='4015' bot=False nick='Alicia - SPAT (10)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817531532180717639 name='Hervé Pierrick' discriminator='9042' bot=False nick="Pierrick - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=429294921447637013 name='Cassie du CJ de Chamarande' discriminator='4125' bot=False nick='Cassie - Chamarande (91)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=812420593580244992 name='eliinaa_mrz' discriminator='0489' bot=False nick="Elina - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=818876857675677741 name='Anne sophie Cluses' discriminator='2450' bot=False nick='Anne - Cluses (74)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=806134269557604373 name='Société Protectrice des Animaux' discriminator='3238' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=791637538618998795 name='Tiâa-Forbach (57)' discriminator='2332' bot=False nick='Tiâa - Forbach (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=812365154184069132 name='Alma CJ de Bordeaux' discriminator='1871' bot=False nick='Alma - Bordeaux (33)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=159985870458322944 name='MEE6' discriminator='4876' bot=True nick='🐱Simon' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=806174108286451764 name='Reale COUCHAUX' discriminator='6300' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817666308996464640 name='Sandrine CJ Rennes' discriminator='2463' bot=False nick='Sandrine - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=824916103918387223 name='Patou' discriminator='8474' bot=False nick='Patou - Pornic (44)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817684166274842654 name='Jean DUQUESNOIS' discriminator='2933' bot=False nick='Jean - Vallérargues (30)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=821726042800390154 name='Valérie CJ Poulainville' discriminator='0191' bot=False nick='Valérie - Poulainville (80)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=777254181034917928 name='Candice' discriminator='2097' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=823524195119792158 name='PPM' discriminator='8874' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=554701108786888754 name='ness' discriminator='9391' bot=False nick="Ines - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=819231783635648543 name='imogen CJ de briancon' discriminator='1398' bot=False nick='Imogen - Briançon (05)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=743880812981911563 name='lilie CJ Saint omer' discriminator='3660' bot=False nick='Lilie - Saint-Omer (62)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=688447791437054061 name='Manon Ricaud' discriminator='6573' bot=False nick='Manon - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=649282683255521305 name='Anaïs CJ de Saint Pierre du Mont' discriminator='1284' bot=False nick='Anaïs - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=826181220836704286 name='Klervia' discriminator='3930' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=811873653066301466 name='Margau CJ de Vaux-le-Pénil' discriminator='1974' bot=False nick='Margau - Vaux-le-Pénil (77)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=803322855290437703 name='Ewen du CJ de Chateaubourg' discriminator='7758' bot=False nick='Ewen - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=818072289346191395 name='Trinity49' discriminator='5916' bot=False nick='Didier - Cholet (49)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=818553720135614496 name='Charlotte du CJ de le Garric' discriminator='9861' bot=False nick='Charlotte - Le Garric (81)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=811656729812664370 name='Hugo CJ Saint Pierre du Mont' discriminator='2618' bot=False nick='Céline - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=811723077301174363 name='Marine CJ de Chateaubourg' discriminator='3546' bot=False nick='Marine - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=717010697120120862 name='Manon CJ orgeval' discriminator='5414' bot=False nick='Manon - Orgeval (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817468032645070909 name='MariaF' discriminator='9993' bot=False nick='Maria - La Roche-sur-Yon (85)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=820687749546901539 name='zines' discriminator='8670' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=387907535019048961 name='Pauline' discriminator='8887' bot=False nick='Pauline - Chateaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=783025428431634463 name='lilou' discriminator='0184' bot=False nick='Lilou - Saint-Omer (62)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=814843381876129834 name='Manon CJ de la Roche sur Yon' discriminator='0140' bot=False nick='Manon - La Roche-sur-Yon (85)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=812337799717584961 name='Luna CJ de Millau' discriminator='7128' bot=False nick='Luna - Millau (12)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817446940492562443 name='Aurore CJ Vaulx le Penil' discriminator='3737' bot=False nick='Aurore - Vaux-le-Pénil (77)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=820389495169876028 name='Elina' discriminator='3472' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=824237075141230593 name='Chloé CJ Luynes' discriminator='7836' bot=False nick='Chloé - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=779255638911221790 name='Clémentine CJ SaintPierreDuMont' discriminator='3516' bot=False nick='Clémentine - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=809826133755428886 name='Ragnarock' discriminator='1491' bot=False nick='Élodie - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817668024613339177 name='Audrey (endadrante 81)' discriminator='4921' bot=False nick='Audrey - Le Garric (81)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=526740097698365440 name='Lgjump' discriminator='1054' bot=False nick='Thomas - Vaux-le-Pénil (77)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=812706223476178956 name='chachou' discriminator='7048' bot=False nick="Charlotte - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=558996910581612545 name='QuizBot' discriminator='0134' bot=True nick='🐶Togo' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=690517117056843836 name='maëlia-j' discriminator='7916' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817502019048439889 name='Virginie' discriminator='0867' bot=False nick='Virginie - Arry (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=294200564357791745 name='Cédric' discriminator='6625' bot=False nick='Cédric - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=814096503575412747 name='Hanna.cnlr' discriminator='2575' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=814809886885937162 name='Lana du CJ de Chamarande' discriminator='4322' bot=False nick='Lana - Chamarande (91)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=812429809950785597 name='Sarah CJ de Chameyrat' discriminator='7571' bot=False nick='Sarah - Chameyrat (19)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=821766847556091944 name='Léandra cj de luynes' discriminator='3188' bot=False nick='Léandra - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=814554700983566356 name='Elsa CJ Lons Le Saunier' discriminator='3355' bot=False nick='Elsa - Lons-le-Saunier (39)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817456457397043241 name='Stephane (Thionville)' discriminator='1753' bot=False nick='Stéphane - Thionville (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=776446881403240458 name='Lucie mages' discriminator='6400' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=818564026237452350 name='Ohana' discriminator='1949' bot=True nick='🐶 Ohana' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=813424879491219456 name='Lily CJ de Rennes' discriminator='3661' bot=False nick='Lily - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817716881950900234 name='Naïs' discriminator='5636' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=818560915817103370 name='caroline enc.CJ Thionville' discriminator='5118' bot=False nick='Caroline - Thionville (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=821799744996769822 name='Owen du CJ de luyne' discriminator='3245' bot=False nick='Owen - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=698528620423151706 name='Valentin CJ vaux-le-pénil' discriminator='8476' bot=False nick='Valentin - Vaux-le-Pénil (77)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=739521549132103712 name='sgodefroy' discriminator='7405' bot=False nick='Stephane - Thionville (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817455331637461033 name='Romane Chateaubourg' discriminator='6316' bot=False nick='Romane - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=797583554988474418 name='Zoé- Forbach (57)' discriminator='7769' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=811574480299491338 name='Lorette CJ Saint Pierre du Mont' discriminator='1730' bot=False nick='Lorette - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=815284094417764383 name='Capucine CJ de Plaisir' discriminator='2186' bot=False nick='Capucine - Plaisir (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=573070802577129473 name="Romain CJ de Yvré l'Évèque" discriminator='9972' bot=False nick="Romain - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=821843675272970272 name='Club jeunes Chamarande' discriminator='6857' bot=False nick='Léa - Chamarande (91)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=831266666486562846 name='lilium' discriminator='2421' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=812420035493625947 name="Mathéa.s de Yvré l'éveque 72" discriminator='3239' bot=False nick="Mathéa.s - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=688137172179615745 name='🌟 「 𝔹𝕒𝕓𝕪 𝕘𝕚𝕣𝕝 」 🌟' discriminator='7001' bot=False nick="Timothé - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=569597210728071210 name='Louve' discriminator='1683' bot=False nick='Laureline - Plaisir (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=819170497132363799 name='Ereann cj vaux le penil' discriminator='2086' bot=False nick='Ereann - Vaux-le-Pénil (77)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=691588451547480076 name='Stéph_of28' discriminator='9983' bot=False nick='Stéphanie - Saint-Omer (62)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=812289741294534718 name='Noelly CJ de Chameyrat' discriminator='1221' bot=False nick='Noelly - Chameyrat (19)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=439791430651609089 name='Repti' discriminator='9965' bot=False nick='Enzo - Saint-Omer (62)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817369610051125309 name='Clémence' discriminator='9498' bot=False nick="Clémence - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=828949602937864202 name='Anne-Sophie - Forbach (57)' discriminator='7869' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=704237474221654086 name='léa' discriminator='3402' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=816646879135793152 name='titouan de poulainville' discriminator='6643' bot=False nick='Titouan - Poulainville (80)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=674885857458651161 name='MemberList' discriminator='4997' bot=True nick='🐶Hachikō' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=818559139415719976 name='KimieCJduGarric' discriminator='7403' bot=False nick='Kimie - Le Garric (81)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=231129972755005440 name='Oyoelle' discriminator='7903' bot=False nick='Elwenn - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=816751853026017361 name='Lony cj poulainville' discriminator='5437' bot=False nick='Lony - Poulainville (80)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=653187728032399391 name='ImnotnathaYT' discriminator='8079' bot=False nick='Nathael - Bordeaux (33)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=821072189080076328 name='Marine du CJ de la Roche sur Yon' discriminator='0978' bot=False nick='Marine - La Roche-sur-Yon (85)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=752240686992064693 name='Meli melo' discriminator='9181' bot=False nick='Meryam - Forbach (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=828320232971829299 name='julie37' discriminator='9767' bot=False nick='Julie - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=683034848981680129 name="lily_blk CJ de yvré l'évêque" discriminator='7445' bot=False nick="Lily - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=766218397536354335 name='Abel_j' discriminator='2508' bot=False nick='Abel - Chamarande (91)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=809820884553826415 name='magic-Tim' discriminator='2385' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=689400323713794078 name='Marie-Agnès' discriminator='5423' bot=False nick='Marie-Agnès - Orgeval (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=811897434225377280 name='Héloïse CJ de Chameyrat' discriminator='5373' bot=False nick='Héloïse - Chameyrat (19)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=689473018740998159 name='Cathy' discriminator='7851' bot=False nick='Cathy - Sarreguemines (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=689815595746590832 name='jtmfort' discriminator='1427' bot=False nick='Lola - Vaux-le-Pénil (77)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=811893356618579978 name='Lily CJ de Rennes' discriminator='3212' bot=False nick='Lily - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=812625585276846130 name='YACINE CJ PLAISIR 78' discriminator='7816' bot=False nick='Yacine - Plaisir (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=822061661564174348 name='Nils05100' discriminator='4521' bot=False nick='Nils - Briançon (05)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=333364261688442890 name='Lucas ²' discriminator='1486' bot=False nick='Lucas - Forbach (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=811688103668219915 name='Lily CJ de Rennes' discriminator='0920' bot=False nick='Lily - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=806174253849378839 name='Kévin DOUANGSAVATH' discriminator='6501' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=812780108036571136 name='Chiara CJ de Niort' discriminator='8059' bot=False nick='Chiara - Niort (79)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=666896278021472287 name='Cassou-edn' discriminator='0209' bot=False nick="Cassandre - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=774024415859834911 name='malena' discriminator='8914' bot=False nick='Maléna - Cholet (49)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=694309330429804545 name='Valentine' discriminator='5125' bot=False nick='Valentine - Saint-Omer (62)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817867946701226003 name='paupau' discriminator='2647' bot=False nick='Pauline - Forbach (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=832180379527282688 name='lilou37' discriminator='1946' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=814861125580881940 name='Léane du CJ de Plaisir' discriminator='1982' bot=False nick='Léane - Plaisir (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=771378220809453589 name='Dotmazy' discriminator='5284' bot=False nick='Thibault - Cj luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=324631108731928587 name='Simple Poll' discriminator='9879' bot=True nick='🐶Laïka' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=826134409349955594 name='Mary-Chateaubourg35' discriminator='3382' bot=False nick='Mary - Chateaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=812399451427307542 name='sarah kervinio Yvré' discriminator='5630' bot=False nick="Sarah - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817494596170416128 name='Dragana' discriminator='8632' bot=False nick='Dragana - Laon (02)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=791638268247801898 name='Lucie - Forbach (57)' discriminator='7764' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=777226843963129926 name='Evangéline' discriminator='9710' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817462125815398411 name='Cécile Encadrante CJ Luynes (37)' discriminator='4741' bot=False nick='Cécile - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=689063301199822971 name='Loane' discriminator='5676' bot=False nick='Loane - Chamarande (91)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=689875189814657053 name='Hélène - Encadrante SPA - Millau' discriminator='0248' bot=False nick='Hélène - Millau (12)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=410138084181671938 name='Aiglor009' discriminator='3918' bot=False nick='Thomas - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=824269174246998076 name='Louna CJ de Luynes' discriminator='1106' bot=False nick='Louna - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=812023228167618601 name='Sylvie CJ St OMER' discriminator='3410' bot=False nick='Sylvie - Saint-Omer (62)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=821332977371185152 name='catherine vitre' discriminator='6716' bot=False nick='Catherine - Vitré (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=811685909669216287 name='Lily CJ de Rennes' discriminator='7358' bot=False nick='Lily - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=820921651343785985 name='Sophie RADIDEAU ROBINE' discriminator='2033' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817630483294060595 name='Catherine Fuseau' discriminator='8144' bot=False nick='Catherine - SPAT (10)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=826888582060179516 name='Laura CJ St Pierre du Mont' discriminator='3104' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=826007429703532545 name='Cassy CJ de Chamarande' discriminator='3125' bot=False nick='Cassy - Chamarande (91)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=725471539365150867 name='Erwan' discriminator='0084' bot=False nick='Erwan - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817456802983575553 name='Alix CJ SPDM' discriminator='4012' bot=False nick='Alix - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=772050348592201729 name='maelys CJ Pornic' discriminator='7949' bot=False nick='Maelys - Pornic (44)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817472074028941322 name='Marinette CJ de Luynes' discriminator='4290' bot=False nick='Marinette - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=614958426849542157 name="Le P'tit Beurre Fou" discriminator='3503' bot=False nick='Eliott - Briançon (05)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=823644993427865690 name='Manonmr' discriminator='6723' bot=False nick='Manon - Le Garric (81)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=713390694806323312 name='Justine' discriminator='8951' bot=False nick='Justine - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=820014965867151370 name='erine du CJ de vaux le penil' discriminator='0120' bot=False nick='Erine - Vaux-le-Pénil (77)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=813532163655729172 name='Kelly CJ De Luynes' discriminator='4055' bot=False nick='Kelly - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=814843246046871604 name='Héléna CJ de Laon' discriminator='0749' bot=False nick='Héléna - Laon (02)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=723818066932269137 name='Marianne' discriminator='0263' bot=False nick='Marianne - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=814539477057011762 name='Clementine CJ de Millau' discriminator='9234' bot=False nick='Clementine - Millau (12)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817494454927491093 name='Maria CJ La Roche sur Yon' discriminator='7686' bot=False nick='Maria - La Roche-sur-Yon (85)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=689831329331675143 name='Marywenn.Pornic(44)' discriminator='1346' bot=False nick='Maryween - Pornic (44)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=765294557252157440 name='Anaël CJ de Cluses' discriminator='7963' bot=False nick='Anaël - Cluses (74)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=818083516234989588 name='Chantale CJ de Plaisir' discriminator='3278' bot=False nick='Chantale - Plaisir (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=818128336185196544 name='Lena Raimbaud' discriminator='9590' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=796103288646926437 name='Garance' discriminator='7603' bot=False nick='Garance - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=690509463924506626 name='nightfox' discriminator='9964' bot=False nick='Esteban - Plaisir (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=819282970023559180 name='ines Cj thionville' discriminator='1353' bot=False nick='Inès - Thionville (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=814469566595596288 name='Lily CJ de Rennes' discriminator='3091' bot=False nick='Lily - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=811576583613579324 name='soizic du CJ de la roche sur yon' discriminator='8969' bot=False nick='Soizic - La Roche-sur-Yon (85)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=717309388830015528 name='Héloïse CJ de Pornic' discriminator='6617' bot=False nick='Héloise - Pornic (44)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=826007033266176011 name='Cassy CJ de Chamarande' discriminator='6404' bot=False nick='Cassy - Chamarande (91)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=825621468679110656 name='Lola du CJ du Garric' discriminator='6051' bot=False nick='Lola - Le Garric (81)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=793473737310601227 name='Alicia CJ de Menois' discriminator='4015' bot=False nick='Alicia - SPAT (10)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817531532180717639 name='Hervé Pierrick' discriminator='9042' bot=False nick="Pierrick - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=429294921447637013 name='Cassie du CJ de Chamarande' discriminator='4125' bot=False nick='Cassie - Chamarande (91)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=812420593580244992 name='eliinaa_mrz' discriminator='0489' bot=False nick="Elina - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=818876857675677741 name='Anne sophie Cluses' discriminator='2450' bot=False nick='Anne - Cluses (74)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=806134269557604373 name='Société Protectrice des Animaux' discriminator='3238' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=791637538618998795 name='Tiâa-Forbach (57)' discriminator='2332' bot=False nick='Tiâa - Forbach (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=812365154184069132 name='Alma CJ de Bordeaux' discriminator='1871' bot=False nick='Alma - Bordeaux (33)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=159985870458322944 name='MEE6' discriminator='4876' bot=True nick='🐱Simon' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=806174108286451764 name='Reale COUCHAUX' discriminator='6300' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817666308996464640 name='Sandrine CJ Rennes' discriminator='2463' bot=False nick='Sandrine - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=824916103918387223 name='Patou' discriminator='8474' bot=False nick='Patou - Pornic (44)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817684166274842654 name='Jean DUQUESNOIS' discriminator='2933' bot=False nick='Jean - Vallérargues (30)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=821726042800390154 name='Valérie CJ Poulainville' discriminator='0191' bot=False nick='Valérie - Poulainville (80)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=777254181034917928 name='Candice' discriminator='2097' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=823524195119792158 name='PPM' discriminator='8874' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=554701108786888754 name='ness' discriminator='9391' bot=False nick="Ines - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=819231783635648543 name='imogen CJ de briancon' discriminator='1398' bot=False nick='Imogen - Briançon (05)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=743880812981911563 name='lilie CJ Saint omer' discriminator='3660' bot=False nick='Lilie - Saint-Omer (62)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=688447791437054061 name='Manon Ricaud' discriminator='6573' bot=False nick='Manon - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=649282683255521305 name='Anaïs CJ de Saint Pierre du Mont' discriminator='1284' bot=False nick='Anaïs - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=826181220836704286 name='Klervia' discriminator='3930' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=811873653066301466 name='Margau CJ de Vaux-le-Pénil' discriminator='1974' bot=False nick='Margau - Vaux-le-Pénil (77)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=803322855290437703 name='Ewen du CJ de Chateaubourg' discriminator='7758' bot=False nick='Ewen - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=818072289346191395 name='Trinity49' discriminator='5916' bot=False nick='Didier - Cholet (49)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=818553720135614496 name='Charlotte du CJ de le Garric' discriminator='9861' bot=False nick='Charlotte - Le Garric (81)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=811656729812664370 name='Hugo CJ Saint Pierre du Mont' discriminator='2618' bot=False nick='Céline - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=811723077301174363 name='Marine CJ de Chateaubourg' discriminator='3546' bot=False nick='Marine - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=717010697120120862 name='Manon CJ orgeval' discriminator='5414' bot=False nick='Manon - Orgeval (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817468032645070909 name='MariaF' discriminator='9993' bot=False nick='Maria - La Roche-sur-Yon (85)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=820687749546901539 name='zines' discriminator='8670' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=387907535019048961 name='Pauline' discriminator='8887' bot=False nick='Pauline - Chateaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=783025428431634463 name='lilou' discriminator='0184' bot=False nick='Lilou - Saint-Omer (62)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=814843381876129834 name='Manon CJ de la Roche sur Yon' discriminator='0140' bot=False nick='Manon - La Roche-sur-Yon (85)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=812337799717584961 name='Luna CJ de Millau' discriminator='7128' bot=False nick='Luna - Millau (12)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817446940492562443 name='Aurore CJ Vaulx le Penil' discriminator='3737' bot=False nick='Aurore - Vaux-le-Pénil (77)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=820389495169876028 name='Elina' discriminator='3472' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=824237075141230593 name='Chloé CJ Luynes' discriminator='7836' bot=False nick='Chloé - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=779255638911221790 name='Clémentine CJ SaintPierreDuMont' discriminator='3516' bot=False nick='Clémentine - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=809826133755428886 name='Ragnarock' discriminator='1491' bot=False nick='Élodie - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817668024613339177 name='Audrey (endadrante 81)' discriminator='4921' bot=False nick='Audrey - Le Garric (81)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=526740097698365440 name='Lgjump' discriminator='1054' bot=False nick='Thomas - Vaux-le-Pénil (77)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=812706223476178956 name='chachou' discriminator='7048' bot=False nick="Charlotte - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=558996910581612545 name='QuizBot' discriminator='0134' bot=True nick='🐶Togo' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=690517117056843836 name='maëlia-j' discriminator='7916' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817502019048439889 name='Virginie' discriminator='0867' bot=False nick='Virginie - Arry (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=294200564357791745 name='Cédric' discriminator='6625' bot=False nick='Cédric - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=814096503575412747 name='Hanna.cnlr' discriminator='2575' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=814809886885937162 name='Lana du CJ de Chamarande' discriminator='4322' bot=False nick='Lana - Chamarande (91)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=812429809950785597 name='Sarah CJ de Chameyrat' discriminator='7571' bot=False nick='Sarah - Chameyrat (19)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=821766847556091944 name='Léandra cj de luynes' discriminator='3188' bot=False nick='Léandra - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=814554700983566356 name='Elsa CJ Lons Le Saunier' discriminator='3355' bot=False nick='Elsa - Lons-le-Saunier (39)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817456457397043241 name='Stephane (Thionville)' discriminator='1753' bot=False nick='Stéphane - Thionville (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=776446881403240458 name='Lucie mages' discriminator='6400' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=818564026237452350 name='Ohana' discriminator='1949' bot=True nick='🐶 Ohana' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=813424879491219456 name='Lily CJ de Rennes' discriminator='3661' bot=False nick='Lily - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817716881950900234 name='Naïs' discriminator='5636' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=818560915817103370 name='caroline enc.CJ Thionville' discriminator='5118' bot=False nick='Caroline - Thionville (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=821799744996769822 name='Owen du CJ de luyne' discriminator='3245' bot=False nick='Owen - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=698528620423151706 name='Valentin CJ vaux-le-pénil' discriminator='8476' bot=False nick='Valentin - Vaux-le-Pénil (77)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=739521549132103712 name='sgodefroy' discriminator='7405' bot=False nick='Stephane - Thionville (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817455331637461033 name='Romane Chateaubourg' discriminator='6316' bot=False nick='Romane - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=797583554988474418 name='Zoé- Forbach (57)' discrimin</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -601,7 +601,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>[&lt;Member id=818564026237452350 name='Ohana' discriminator='1949' bot=True nick='🐶 Ohana' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=818564026237452350 name='Ohana' discriminator='1949' bot=True nick='🐶 Ohana' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -664,7 +664,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>[&lt;Member id=324631108731928587 name='Simple Poll' discriminator='9879' bot=True nick='🐶Laïka' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=324631108731928587 name='Simple Poll' discriminator='9879' bot=True nick='🐶Laïka' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -727,7 +727,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>[&lt;Member id=159985870458322944 name='MEE6' discriminator='4876' bot=True nick='🐱Simon' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=159985870458322944 name='MEE6' discriminator='4876' bot=True nick='🐱Simon' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -790,7 +790,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>[&lt;Member id=558996910581612545 name='QuizBot' discriminator='0134' bot=True nick='🐶Togo' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=558996910581612545 name='QuizBot' discriminator='0134' bot=True nick='🐶Togo' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -853,7 +853,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>[&lt;Member id=674885857458651161 name='MemberList' discriminator='4997' bot=True nick='🐶Hachikō' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=674885857458651161 name='MemberList' discriminator='4997' bot=True nick='🐶Hachikō' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -916,7 +916,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>[&lt;Member id=674885857458651161 name='MemberList' discriminator='4997' bot=True nick='🐶Hachikō' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=324631108731928587 name='Simple Poll' discriminator='9879' bot=True nick='🐶Laïka' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=159985870458322944 name='MEE6' discriminator='4876' bot=True nick='🐱Simon' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=558996910581612545 name='QuizBot' discriminator='0134' bot=True nick='🐶Togo' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=818564026237452350 name='Ohana' discriminator='1949' bot=True nick='🐶 Ohana' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=674885857458651161 name='MemberList' discriminator='4997' bot=True nick='🐶Hachikō' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=324631108731928587 name='Simple Poll' discriminator='9879' bot=True nick='🐶Laïka' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=159985870458322944 name='MEE6' discriminator='4876' bot=True nick='🐱Simon' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=558996910581612545 name='QuizBot' discriminator='0134' bot=True nick='🐶Togo' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=818564026237452350 name='Ohana' discriminator='1949' bot=True nick='🐶 Ohana' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -975,7 +975,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>[&lt;Member id=573070802577129473 name="Romain CJ de Yvré l'Évèque" discriminator='9972' bot=False nick="Romain - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=812420035493625947 name="Mathéa.s de Yvré l'éveque 72" discriminator='3239' bot=False nick="Mathéa.s - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=688137172179615745 name='🌟 「 𝔹𝕒𝕓𝕪 𝕘𝕚𝕣𝕝 」 🌟' discriminator='7001' bot=False nick="Timothé - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817369610051125309 name='Clémence' discriminator='9498' bot=False nick="Clémence - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=683034848981680129 name="lily_blk CJ de yvré l'évêque" discriminator='7445' bot=False nick="Lily - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=666896278021472287 name='Cassou-edn' discriminator='0209' bot=False nick="Cassandre - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=812399451427307542 name='sarah kervinio Yvré' discriminator='5630' bot=False nick="Sarah - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817531532180717639 name='Hervé Pierrick' discriminator='9042' bot=False nick="Pierrick - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=812420593580244992 name='eliinaa_mrz' discriminator='0489' bot=False nick="Elina - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=554701108786888754 name='ness' discriminator='9391' bot=False nick="Ines - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=812706223476178956 name='chachou' discriminator='7048' bot=False nick="Charlotte - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=573070802577129473 name="Romain CJ de Yvré l'Évèque" discriminator='9972' bot=False nick="Romain - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=812420035493625947 name="Mathéa.s de Yvré l'éveque 72" discriminator='3239' bot=False nick="Mathéa.s - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=688137172179615745 name='🌟 「 𝔹𝕒𝕓𝕪 𝕘𝕚𝕣𝕝 」 🌟' discriminator='7001' bot=False nick="Timothé - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817369610051125309 name='Clémence' discriminator='9498' bot=False nick="Clémence - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=683034848981680129 name="lily_blk CJ de yvré l'évêque" discriminator='7445' bot=False nick="Lily - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=666896278021472287 name='Cassou-edn' discriminator='0209' bot=False nick="Cassandre - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=812399451427307542 name='sarah kervinio Yvré' discriminator='5630' bot=False nick="Sarah - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817531532180717639 name='Hervé Pierrick' discriminator='9042' bot=False nick="Pierrick - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=812420593580244992 name='eliinaa_mrz' discriminator='0489' bot=False nick="Elina - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=554701108786888754 name='ness' discriminator='9391' bot=False nick="Ines - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=812706223476178956 name='chachou' discriminator='7048' bot=False nick="Charlotte - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -1034,7 +1034,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>[&lt;Member id=821332977371185152 name='catherine vitre' discriminator='6716' bot=False nick='Catherine - Vitré (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=821332977371185152 name='catherine vitre' discriminator='6716' bot=False nick='Catherine - Vitré (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
@@ -1093,7 +1093,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>[&lt;Member id=819170497132363799 name='Ereann cj vaux le penil' discriminator='2086' bot=False nick='Ereann - Vaux-le-Pénil (77)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=689815595746590832 name='jtmfort' discriminator='1427' bot=False nick='Lola - Vaux-le-Pénil (77)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=820014965867151370 name='erine du CJ de vaux le penil' discriminator='0120' bot=False nick='Erine - Vaux-le-Pénil (77)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=811873653066301466 name='Margau CJ de Vaux-le-Pénil' discriminator='1974' bot=False nick='Margau - Vaux-le-Pénil (77)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817446940492562443 name='Aurore CJ Vaulx le Penil' discriminator='3737' bot=False nick='Aurore - Vaux-le-Pénil (77)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=526740097698365440 name='Lgjump' discriminator='1054' bot=False nick='Thomas - Vaux-le-Pénil (77)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=698528620423151706 name='Valentin CJ vaux-le-pénil' discriminator='8476' bot=False nick='Valentin - Vaux-le-Pénil (77)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=819170497132363799 name='Ereann cj vaux le penil' discriminator='2086' bot=False nick='Ereann - Vaux-le-Pénil (77)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=689815595746590832 name='jtmfort' discriminator='1427' bot=False nick='Lola - Vaux-le-Pénil (77)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=820014965867151370 name='erine du CJ de vaux le penil' discriminator='0120' bot=False nick='Erine - Vaux-le-Pénil (77)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=811873653066301466 name='Margau CJ de Vaux-le-Pénil' discriminator='1974' bot=False nick='Margau - Vaux-le-Pénil (77)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817446940492562443 name='Aurore CJ Vaulx le Penil' discriminator='3737' bot=False nick='Aurore - Vaux-le-Pénil (77)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=526740097698365440 name='Lgjump' discriminator='1054' bot=False nick='Thomas - Vaux-le-Pénil (77)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=698528620423151706 name='Valentin CJ vaux-le-pénil' discriminator='8476' bot=False nick='Valentin - Vaux-le-Pénil (77)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -1152,7 +1152,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>[&lt;Member id=817684166274842654 name='Jean DUQUESNOIS' discriminator='2933' bot=False nick='Jean - Vallérargues (30)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=817684166274842654 name='Jean DUQUESNOIS' discriminator='2933' bot=False nick='Jean - Vallérargues (30)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -1211,7 +1211,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>[&lt;Member id=819282970023559180 name='ines Cj thionville' discriminator='1353' bot=False nick='Inès - Thionville (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817456457397043241 name='Stephane (Thionville)' discriminator='1753' bot=False nick='Stéphane - Thionville (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=818560915817103370 name='caroline enc.CJ Thionville' discriminator='5118' bot=False nick='Caroline - Thionville (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=739521549132103712 name='sgodefroy' discriminator='7405' bot=False nick='Stephane - Thionville (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=819282970023559180 name='ines Cj thionville' discriminator='1353' bot=False nick='Inès - Thionville (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817456457397043241 name='Stephane (Thionville)' discriminator='1753' bot=False nick='Stéphane - Thionville (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=818560915817103370 name='caroline enc.CJ Thionville' discriminator='5118' bot=False nick='Caroline - Thionville (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=739521549132103712 name='sgodefroy' discriminator='7405' bot=False nick='Stephane - Thionville (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
@@ -1270,7 +1270,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>[&lt;Member id=817630483294060595 name='Catherine Fuseau' discriminator='8144' bot=False nick='Catherine - SPAT (10)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=793473737310601227 name='Alicia CJ de Menois' discriminator='4015' bot=False nick='Alicia - SPAT (10)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=817630483294060595 name='Catherine Fuseau' discriminator='8144' bot=False nick='Catherine - SPAT (10)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=793473737310601227 name='Alicia CJ de Menois' discriminator='4015' bot=False nick='Alicia - SPAT (10)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
@@ -1329,7 +1329,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>[&lt;Member id=689473018740998159 name='Cathy' discriminator='7851' bot=False nick='Cathy - Sarreguemines (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=689473018740998159 name='Cathy' discriminator='7851' bot=False nick='Cathy - Sarreguemines (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -1388,7 +1388,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>[&lt;Member id=811574480299491338 name='Lorette CJ Saint Pierre du Mont' discriminator='1730' bot=False nick='Lorette - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=826888582060179516 name='Laura CJ St Pierre du Mont' discriminator='3104' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817456802983575553 name='Alix CJ SPDM' discriminator='4012' bot=False nick='Alix - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=796103288646926437 name='Garance' discriminator='7603' bot=False nick='Garance - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=688447791437054061 name='Manon Ricaud' discriminator='6573' bot=False nick='Manon - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=649282683255521305 name='Anaïs CJ de Saint Pierre du Mont' discriminator='1284' bot=False nick='Anaïs - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=811656729812664370 name='Hugo CJ Saint Pierre du Mont' discriminator='2618' bot=False nick='Céline - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=779255638911221790 name='Clémentine CJ SaintPierreDuMont' discriminator='3516' bot=False nick='Clémentine - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=811574480299491338 name='Lorette CJ Saint Pierre du Mont' discriminator='1730' bot=False nick='Lorette - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=826888582060179516 name='Laura CJ St Pierre du Mont' discriminator='3104' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817456802983575553 name='Alix CJ SPDM' discriminator='4012' bot=False nick='Alix - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=796103288646926437 name='Garance' discriminator='7603' bot=False nick='Garance - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=688447791437054061 name='Manon Ricaud' discriminator='6573' bot=False nick='Manon - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=649282683255521305 name='Anaïs CJ de Saint Pierre du Mont' discriminator='1284' bot=False nick='Anaïs - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=811656729812664370 name='Hugo CJ Saint Pierre du Mont' discriminator='2618' bot=False nick='Céline - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=779255638911221790 name='Clémentine CJ SaintPierreDuMont' discriminator='3516' bot=False nick='Clémentine - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -1447,7 +1447,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>[&lt;Member id=691588451547480076 name='Stéph_of28' discriminator='9983' bot=False nick='Stéphanie - Saint-Omer (62)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=439791430651609089 name='Repti' discriminator='9965' bot=False nick='Enzo - Saint-Omer (62)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=694309330429804545 name='Valentine' discriminator='5125' bot=False nick='Valentine - Saint-Omer (62)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=812023228167618601 name='Sylvie CJ St OMER' discriminator='3410' bot=False nick='Sylvie - Saint-Omer (62)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=743880812981911563 name='lilie CJ Saint omer' discriminator='3660' bot=False nick='Lilie - Saint-Omer (62)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=783025428431634463 name='lilou' discriminator='0184' bot=False nick='Lilou - Saint-Omer (62)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=691588451547480076 name='Stéph_of28' discriminator='9983' bot=False nick='Stéphanie - Saint-Omer (62)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=439791430651609089 name='Repti' discriminator='9965' bot=False nick='Enzo - Saint-Omer (62)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=694309330429804545 name='Valentine' discriminator='5125' bot=False nick='Valentine - Saint-Omer (62)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=812023228167618601 name='Sylvie CJ St OMER' discriminator='3410' bot=False nick='Sylvie - Saint-Omer (62)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=743880812981911563 name='lilie CJ Saint omer' discriminator='3660' bot=False nick='Lilie - Saint-Omer (62)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=783025428431634463 name='lilou' discriminator='0184' bot=False nick='Lilou - Saint-Omer (62)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -1506,7 +1506,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>[&lt;Member id=821072189080076328 name='Marine du CJ de la Roche sur Yon' discriminator='0978' bot=False nick='Marine - La Roche-sur-Yon (85)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817494454927491093 name='Maria CJ La Roche sur Yon' discriminator='7686' bot=False nick='Maria - La Roche-sur-Yon (85)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=811576583613579324 name='soizic du CJ de la roche sur yon' discriminator='8969' bot=False nick='Soizic - La Roche-sur-Yon (85)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817468032645070909 name='MariaF' discriminator='9993' bot=False nick='Maria - La Roche-sur-Yon (85)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=814843381876129834 name='Manon CJ de la Roche sur Yon' discriminator='0140' bot=False nick='Manon - La Roche-sur-Yon (85)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=821072189080076328 name='Marine du CJ de la Roche sur Yon' discriminator='0978' bot=False nick='Marine - La Roche-sur-Yon (85)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817494454927491093 name='Maria CJ La Roche sur Yon' discriminator='7686' bot=False nick='Maria - La Roche-sur-Yon (85)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=811576583613579324 name='soizic du CJ de la roche sur yon' discriminator='8969' bot=False nick='Soizic - La Roche-sur-Yon (85)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817468032645070909 name='MariaF' discriminator='9993' bot=False nick='Maria - La Roche-sur-Yon (85)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=814843381876129834 name='Manon CJ de la Roche sur Yon' discriminator='0140' bot=False nick='Manon - La Roche-sur-Yon (85)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -1565,7 +1565,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>[&lt;Member id=811893356618579978 name='Lily CJ de Rennes' discriminator='3212' bot=False nick='Lily - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=811688103668219915 name='Lily CJ de Rennes' discriminator='0920' bot=False nick='Lily - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=410138084181671938 name='Aiglor009' discriminator='3918' bot=False nick='Thomas - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=811685909669216287 name='Lily CJ de Rennes' discriminator='7358' bot=False nick='Lily - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=814469566595596288 name='Lily CJ de Rennes' discriminator='3091' bot=False nick='Lily - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=294200564357791745 name='Cédric' discriminator='6625' bot=False nick='Cédric - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=813424879491219456 name='Lily CJ de Rennes' discriminator='3661' bot=False nick='Lily - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=811893356618579978 name='Lily CJ de Rennes' discriminator='3212' bot=False nick='Lily - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=811688103668219915 name='Lily CJ de Rennes' discriminator='0920' bot=False nick='Lily - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=410138084181671938 name='Aiglor009' discriminator='3918' bot=False nick='Thomas - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=811685909669216287 name='Lily CJ de Rennes' discriminator='7358' bot=False nick='Lily - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=814469566595596288 name='Lily CJ de Rennes' discriminator='3091' bot=False nick='Lily - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=294200564357791745 name='Cédric' discriminator='6625' bot=False nick='Cédric - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=813424879491219456 name='Lily CJ de Rennes' discriminator='3661' bot=False nick='Lily - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
@@ -1624,7 +1624,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>[&lt;Member id=818559139415719976 name='KimieCJduGarric' discriminator='7403' bot=False nick='Kimie - Le Garric (81)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=823644993427865690 name='Manonmr' discriminator='6723' bot=False nick='Manon - Le Garric (81)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=825621468679110656 name='Lola du CJ du Garric' discriminator='6051' bot=False nick='Lola - Le Garric (81)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=818553720135614496 name='Charlotte du CJ de le Garric' discriminator='9861' bot=False nick='Charlotte - Le Garric (81)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817668024613339177 name='Audrey (endadrante 81)' discriminator='4921' bot=False nick='Audrey - Le Garric (81)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=818559139415719976 name='KimieCJduGarric' discriminator='7403' bot=False nick='Kimie - Le Garric (81)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=823644993427865690 name='Manonmr' discriminator='6723' bot=False nick='Manon - Le Garric (81)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=825621468679110656 name='Lola du CJ du Garric' discriminator='6051' bot=False nick='Lola - Le Garric (81)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=818553720135614496 name='Charlotte du CJ de le Garric' discriminator='9861' bot=False nick='Charlotte - Le Garric (81)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817668024613339177 name='Audrey (endadrante 81)' discriminator='4921' bot=False nick='Audrey - Le Garric (81)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
@@ -1683,7 +1683,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>[&lt;Member id=772050348592201729 name='maelys CJ Pornic' discriminator='7949' bot=False nick='Maelys - Pornic (44)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=689831329331675143 name='Marywenn.Pornic(44)' discriminator='1346' bot=False nick='Maryween - Pornic (44)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=717309388830015528 name='Héloïse CJ de Pornic' discriminator='6617' bot=False nick='Héloise - Pornic (44)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=824916103918387223 name='Patou' discriminator='8474' bot=False nick='Patou - Pornic (44)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=772050348592201729 name='maelys CJ Pornic' discriminator='7949' bot=False nick='Maelys - Pornic (44)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=689831329331675143 name='Marywenn.Pornic(44)' discriminator='1346' bot=False nick='Maryween - Pornic (44)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=717309388830015528 name='Héloïse CJ de Pornic' discriminator='6617' bot=False nick='Héloise - Pornic (44)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=824916103918387223 name='Patou' discriminator='8474' bot=False nick='Patou - Pornic (44)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
@@ -1742,7 +1742,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>[&lt;Member id=815284094417764383 name='Capucine CJ de Plaisir' discriminator='2186' bot=False nick='Capucine - Plaisir (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=569597210728071210 name='Louve' discriminator='1683' bot=False nick='Laureline - Plaisir (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=812625585276846130 name='YACINE CJ PLAISIR 78' discriminator='7816' bot=False nick='Yacine - Plaisir (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=814861125580881940 name='Léane du CJ de Plaisir' discriminator='1982' bot=False nick='Léane - Plaisir (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=818083516234989588 name='Chantale CJ de Plaisir' discriminator='3278' bot=False nick='Chantale - Plaisir (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=690509463924506626 name='nightfox' discriminator='9964' bot=False nick='Esteban - Plaisir (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=815284094417764383 name='Capucine CJ de Plaisir' discriminator='2186' bot=False nick='Capucine - Plaisir (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=569597210728071210 name='Louve' discriminator='1683' bot=False nick='Laureline - Plaisir (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=812625585276846130 name='YACINE CJ PLAISIR 78' discriminator='7816' bot=False nick='Yacine - Plaisir (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=814861125580881940 name='Léane du CJ de Plaisir' discriminator='1982' bot=False nick='Léane - Plaisir (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=818083516234989588 name='Chantale CJ de Plaisir' discriminator='3278' bot=False nick='Chantale - Plaisir (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=690509463924506626 name='nightfox' discriminator='9964' bot=False nick='Esteban - Plaisir (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
@@ -1801,7 +1801,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>[&lt;Member id=816646879135793152 name='titouan de poulainville' discriminator='6643' bot=False nick='Titouan - Poulainville (80)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=816751853026017361 name='Lony cj poulainville' discriminator='5437' bot=False nick='Lony - Poulainville (80)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=821726042800390154 name='Valérie CJ Poulainville' discriminator='0191' bot=False nick='Valérie - Poulainville (80)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=816646879135793152 name='titouan de poulainville' discriminator='6643' bot=False nick='Titouan - Poulainville (80)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=816751853026017361 name='Lony cj poulainville' discriminator='5437' bot=False nick='Lony - Poulainville (80)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=821726042800390154 name='Valérie CJ Poulainville' discriminator='0191' bot=False nick='Valérie - Poulainville (80)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
@@ -1860,7 +1860,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>[&lt;Member id=689400323713794078 name='Marie-Agnès' discriminator='5423' bot=False nick='Marie-Agnès - Orgeval (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=717010697120120862 name='Manon CJ orgeval' discriminator='5414' bot=False nick='Manon - Orgeval (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=689400323713794078 name='Marie-Agnès' discriminator='5423' bot=False nick='Marie-Agnès - Orgeval (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=717010697120120862 name='Manon CJ orgeval' discriminator='5414' bot=False nick='Manon - Orgeval (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -1919,7 +1919,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>[&lt;Member id=812780108036571136 name='Chiara CJ de Niort' discriminator='8059' bot=False nick='Chiara - Niort (79)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=812780108036571136 name='Chiara CJ de Niort' discriminator='8059' bot=False nick='Chiara - Niort (79)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
@@ -1978,7 +1978,7 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>[&lt;Member id=689875189814657053 name='Hélène - Encadrante SPA - Millau' discriminator='0248' bot=False nick='Hélène - Millau (12)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=814539477057011762 name='Clementine CJ de Millau' discriminator='9234' bot=False nick='Clementine - Millau (12)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=812337799717584961 name='Luna CJ de Millau' discriminator='7128' bot=False nick='Luna - Millau (12)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=689875189814657053 name='Hélène - Encadrante SPA - Millau' discriminator='0248' bot=False nick='Hélène - Millau (12)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=814539477057011762 name='Clementine CJ de Millau' discriminator='9234' bot=False nick='Clementine - Millau (12)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=812337799717584961 name='Luna CJ de Millau' discriminator='7128' bot=False nick='Luna - Millau (12)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
@@ -2037,7 +2037,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>[&lt;Member id=828320232971829299 name='julie37' discriminator='9767' bot=False nick='Julie - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817462125815398411 name='Cécile Encadrante CJ Luynes (37)' discriminator='4741' bot=False nick='Cécile - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=824269174246998076 name='Louna CJ de Luynes' discriminator='1106' bot=False nick='Louna - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817472074028941322 name='Marinette CJ de Luynes' discriminator='4290' bot=False nick='Marinette - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=813532163655729172 name='Kelly CJ De Luynes' discriminator='4055' bot=False nick='Kelly - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=723818066932269137 name='Marianne' discriminator='0263' bot=False nick='Marianne - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=824237075141230593 name='Chloé CJ Luynes' discriminator='7836' bot=False nick='Chloé - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=821766847556091944 name='Léandra cj de luynes' discriminator='3188' bot=False nick='Léandra - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=821799744996769822 name='Owen du CJ de luyne' discriminator='3245' bot=False nick='Owen - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=828320232971829299 name='julie37' discriminator='9767' bot=False nick='Julie - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=771378220809453589 name='Dotmazy' discriminator='5284' bot=False nick='Thibault - Cj luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817462125815398411 name='Cécile Encadrante CJ Luynes (37)' discriminator='4741' bot=False nick='Cécile - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=824269174246998076 name='Louna CJ de Luynes' discriminator='1106' bot=False nick='Louna - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817472074028941322 name='Marinette CJ de Luynes' discriminator='4290' bot=False nick='Marinette - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=813532163655729172 name='Kelly CJ De Luynes' discriminator='4055' bot=False nick='Kelly - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=723818066932269137 name='Marianne' discriminator='0263' bot=False nick='Marianne - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=824237075141230593 name='Chloé CJ Luynes' discriminator='7836' bot=False nick='Chloé - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=821766847556091944 name='Léandra cj de luynes' discriminator='3188' bot=False nick='Léandra - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=821799744996769822 name='Owen du CJ de luyne' discriminator='3245' bot=False nick='Owen - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -2096,7 +2096,7 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>[&lt;Member id=814554700983566356 name='Elsa CJ Lons Le Saunier' discriminator='3355' bot=False nick='Elsa - Lons-le-Saunier (39)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=814554700983566356 name='Elsa CJ Lons Le Saunier' discriminator='3355' bot=False nick='Elsa - Lons-le-Saunier (39)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
@@ -2214,7 +2214,7 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>[&lt;Member id=817494596170416128 name='Dragana' discriminator='8632' bot=False nick='Dragana - Laon (02)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=814843246046871604 name='Héléna CJ de Laon' discriminator='0749' bot=False nick='Héléna - Laon (02)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=817494596170416128 name='Dragana' discriminator='8632' bot=False nick='Dragana - Laon (02)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=814843246046871604 name='Héléna CJ de Laon' discriminator='0749' bot=False nick='Héléna - Laon (02)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
@@ -2332,7 +2332,7 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>[&lt;Member id=828949602937864202 name='Anne-Sophie - Forbach (57)' discriminator='7869' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=752240686992064693 name='Meli melo' discriminator='9181' bot=False nick='Meryam - Forbach (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=333364261688442890 name='Lucas ²' discriminator='1486' bot=False nick='Lucas - Forbach (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817867946701226003 name='paupau' discriminator='2647' bot=False nick='Pauline - Forbach (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=791638268247801898 name='Lucie - Forbach (57)' discriminator='7764' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=791637538618998795 name='Tiâa-Forbach (57)' discriminator='2332' bot=False nick='Tiâa - Forbach (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=797583554988474418 name='Zoé- Forbach (57)' discriminator='7769' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=828949602937864202 name='Anne-Sophie - Forbach (57)' discriminator='7869' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=752240686992064693 name='Meli melo' discriminator='9181' bot=False nick='Meryam - Forbach (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=333364261688442890 name='Lucas ²' discriminator='1486' bot=False nick='Lucas - Forbach (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817867946701226003 name='paupau' discriminator='2647' bot=False nick='Pauline - Forbach (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=791638268247801898 name='Lucie - Forbach (57)' discriminator='7764' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=791637538618998795 name='Tiâa-Forbach (57)' discriminator='2332' bot=False nick='Tiâa - Forbach (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=797583554988474418 name='Zoé- Forbach (57)' discriminator='7769' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
@@ -2450,7 +2450,7 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>[&lt;Member id=765294557252157440 name='Anaël CJ de Cluses' discriminator='7963' bot=False nick='Anaël - Cluses (74)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=818876857675677741 name='Anne sophie Cluses' discriminator='2450' bot=False nick='Anne - Cluses (74)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=765294557252157440 name='Anaël CJ de Cluses' discriminator='7963' bot=False nick='Anaël - Cluses (74)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=818876857675677741 name='Anne sophie Cluses' discriminator='2450' bot=False nick='Anne - Cluses (74)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
@@ -2509,7 +2509,7 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>[&lt;Member id=774024415859834911 name='malena' discriminator='8914' bot=False nick='Maléna - Cholet (49)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=818072289346191395 name='Trinity49' discriminator='5916' bot=False nick='Didier - Cholet (49)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=774024415859834911 name='malena' discriminator='8914' bot=False nick='Maléna - Cholet (49)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=818072289346191395 name='Trinity49' discriminator='5916' bot=False nick='Didier - Cholet (49)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
@@ -2568,7 +2568,7 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>[&lt;Member id=231129972755005440 name='Oyoelle' discriminator='7903' bot=False nick='Elwenn - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=826134409349955594 name='Mary-Chateaubourg35' discriminator='3382' bot=False nick='Mary - Chateaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=725471539365150867 name='Erwan' discriminator='0084' bot=False nick='Erwan - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=713390694806323312 name='Justine' discriminator='8951' bot=False nick='Justine - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=803322855290437703 name='Ewen du CJ de Chateaubourg' discriminator='7758' bot=False nick='Ewen - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=811723077301174363 name='Marine CJ de Chateaubourg' discriminator='3546' bot=False nick='Marine - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=387907535019048961 name='Pauline' discriminator='8887' bot=False nick='Pauline - Chateaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=809826133755428886 name='Ragnarock' discriminator='1491' bot=False nick='Élodie - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817455331637461033 name='Romane Chateaubourg' discriminator='6316' bot=False nick='Romane - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=231129972755005440 name='Oyoelle' discriminator='7903' bot=False nick='Elwenn - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=826134409349955594 name='Mary-Chateaubourg35' discriminator='3382' bot=False nick='Mary - Chateaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=725471539365150867 name='Erwan' discriminator='0084' bot=False nick='Erwan - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=713390694806323312 name='Justine' discriminator='8951' bot=False nick='Justine - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=803322855290437703 name='Ewen du CJ de Chateaubourg' discriminator='7758' bot=False nick='Ewen - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=811723077301174363 name='Marine CJ de Chateaubourg' discriminator='3546' bot=False nick='Marine - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=387907535019048961 name='Pauline' discriminator='8887' bot=False nick='Pauline - Chateaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=809826133755428886 name='Ragnarock' discriminator='1491' bot=False nick='Élodie - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817455331637461033 name='Romane Chateaubourg' discriminator='6316' bot=False nick='Romane - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
@@ -2627,7 +2627,7 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>[&lt;Member id=812289741294534718 name='Noelly CJ de Chameyrat' discriminator='1221' bot=False nick='Noelly - Chameyrat (19)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=811897434225377280 name='Héloïse CJ de Chameyrat' discriminator='5373' bot=False nick='Héloïse - Chameyrat (19)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=812429809950785597 name='Sarah CJ de Chameyrat' discriminator='7571' bot=False nick='Sarah - Chameyrat (19)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=812289741294534718 name='Noelly CJ de Chameyrat' discriminator='1221' bot=False nick='Noelly - Chameyrat (19)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=811897434225377280 name='Héloïse CJ de Chameyrat' discriminator='5373' bot=False nick='Héloïse - Chameyrat (19)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=812429809950785597 name='Sarah CJ de Chameyrat' discriminator='7571' bot=False nick='Sarah - Chameyrat (19)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
@@ -2686,7 +2686,7 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>[&lt;Member id=821843675272970272 name='Club jeunes Chamarande' discriminator='6857' bot=False nick='Léa - Chamarande (91)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=766218397536354335 name='Abel_j' discriminator='2508' bot=False nick='Abel - Chamarande (91)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=689063301199822971 name='Loane' discriminator='5676' bot=False nick='Loane - Chamarande (91)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=826007429703532545 name='Cassy CJ de Chamarande' discriminator='3125' bot=False nick='Cassy - Chamarande (91)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=826007033266176011 name='Cassy CJ de Chamarande' discriminator='6404' bot=False nick='Cassy - Chamarande (91)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=429294921447637013 name='Cassie du CJ de Chamarande' discriminator='4125' bot=False nick='Cassie - Chamarande (91)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=814809886885937162 name='Lana du CJ de Chamarande' discriminator='4322' bot=False nick='Lana - Chamarande (91)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=821843675272970272 name='Club jeunes Chamarande' discriminator='6857' bot=False nick='Léa - Chamarande (91)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=766218397536354335 name='Abel_j' discriminator='2508' bot=False nick='Abel - Chamarande (91)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=689063301199822971 name='Loane' discriminator='5676' bot=False nick='Loane - Chamarande (91)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=826007429703532545 name='Cassy CJ de Chamarande' discriminator='3125' bot=False nick='Cassy - Chamarande (91)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=826007033266176011 name='Cassy CJ de Chamarande' discriminator='6404' bot=False nick='Cassy - Chamarande (91)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=429294921447637013 name='Cassie du CJ de Chamarande' discriminator='4125' bot=False nick='Cassie - Chamarande (91)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=814809886885937162 name='Lana du CJ de Chamarande' discriminator='4322' bot=False nick='Lana - Chamarande (91)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
@@ -2745,7 +2745,7 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>[&lt;Member id=822061661564174348 name='Nils05100' discriminator='4521' bot=False nick='Nils - Briançon (05)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=614958426849542157 name="Le P'tit Beurre Fou" discriminator='3503' bot=False nick='Eliott - Briançon (05)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=819231783635648543 name='imogen CJ de briancon' discriminator='1398' bot=False nick='Imogen - Briançon (05)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=822061661564174348 name='Nils05100' discriminator='4521' bot=False nick='Nils - Briançon (05)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=614958426849542157 name="Le P'tit Beurre Fou" discriminator='3503' bot=False nick='Eliott - Briançon (05)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=819231783635648543 name='imogen CJ de briancon' discriminator='1398' bot=False nick='Imogen - Briançon (05)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
@@ -2804,7 +2804,7 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>[&lt;Member id=653187728032399391 name='ImnotnathaYT' discriminator='8079' bot=False nick='Nathael - Bordeaux (33)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=812365154184069132 name='Alma CJ de Bordeaux' discriminator='1871' bot=False nick='Alma - Bordeaux (33)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=653187728032399391 name='ImnotnathaYT' discriminator='8079' bot=False nick='Nathael - Bordeaux (33)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=812365154184069132 name='Alma CJ de Bordeaux' discriminator='1871' bot=False nick='Alma - Bordeaux (33)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
@@ -2863,7 +2863,7 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>[&lt;Member id=817502019048439889 name='Virginie' discriminator='0867' bot=False nick='Virginie - Arry (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=817502019048439889 name='Virginie' discriminator='0867' bot=False nick='Virginie - Arry (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
@@ -2981,7 +2981,7 @@
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>[&lt;Member id=806174253849378839 name='Kévin DOUANGSAVATH' discriminator='6501' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=806134269557604373 name='Société Protectrice des Animaux' discriminator='3238' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=806174108286451764 name='Reale COUCHAUX' discriminator='6300' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=806174253849378839 name='Kévin DOUANGSAVATH' discriminator='6501' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=806134269557604373 name='Société Protectrice des Animaux' discriminator='3238' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=806174108286451764 name='Reale COUCHAUX' discriminator='6300' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
@@ -3040,7 +3040,7 @@
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>[&lt;Member id=831266666486562846 name='lilium' discriminator='2421' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=704237474221654086 name='léa' discriminator='3402' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=809820884553826415 name='magic-Tim' discriminator='2385' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=832180379527282688 name='lilou37' discriminator='1946' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=777226843963129926 name='Evangéline' discriminator='9710' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=820921651343785985 name='Sophie RADIDEAU ROBINE' discriminator='2033' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=818128336185196544 name='Lena Raimbaud' discriminator='9590' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817666308996464640 name='Sandrine CJ Rennes' discriminator='2463' bot=False nick='Sandrine - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=777254181034917928 name='Candice' discriminator='2097' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=823524195119792158 name='PPM' discriminator='8874' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=826181220836704286 name='Klervia' discriminator='3930' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=820687749546901539 name='zines' discriminator='8670' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=820389495169876028 name='Elina' discriminator='3472' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=690517117056843836 name='maëlia-j' discriminator='7916' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=814096503575412747 name='Hanna.cnlr' discriminator='2575' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=776446881403240458 name='Lucie mages' discriminator='6400' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817716881950900234 name='Naïs' discriminator='5636' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=831266666486562846 name='lilium' discriminator='2421' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=704237474221654086 name='léa' discriminator='3402' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=809820884553826415 name='magic-Tim' discriminator='2385' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=832180379527282688 name='lilou37' discriminator='1946' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=777226843963129926 name='Evangéline' discriminator='9710' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=820921651343785985 name='Sophie RADIDEAU ROBINE' discriminator='2033' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=818128336185196544 name='Lena Raimbaud' discriminator='9590' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817666308996464640 name='Sandrine CJ Rennes' discriminator='2463' bot=False nick='Sandrine - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=777254181034917928 name='Candice' discriminator='2097' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=823524195119792158 name='PPM' discriminator='8874' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=826181220836704286 name='Klervia' discriminator='3930' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=820687749546901539 name='zines' discriminator='8670' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=820389495169876028 name='Elina' discriminator='3472' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=690517117056843836 name='maëlia-j' discriminator='7916' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=814096503575412747 name='Hanna.cnlr' discriminator='2575' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=776446881403240458 name='Lucie mages' discriminator='6400' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817716881950900234 name='Naïs' discriminator='5636' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
@@ -3099,7 +3099,7 @@
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>[&lt;Member id=811574480299491338 name='Lorette CJ Saint Pierre du Mont' discriminator='1730' bot=False nick='Lorette - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=815284094417764383 name='Capucine CJ de Plaisir' discriminator='2186' bot=False nick='Capucine - Plaisir (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=573070802577129473 name="Romain CJ de Yvré l'Évèque" discriminator='9972' bot=False nick="Romain - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=812420035493625947 name="Mathéa.s de Yvré l'éveque 72" discriminator='3239' bot=False nick="Mathéa.s - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=688137172179615745 name='🌟 「 𝔹𝕒𝕓𝕪 𝕘𝕚𝕣𝕝 」 🌟' discriminator='7001' bot=False nick="Timothé - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=569597210728071210 name='Louve' discriminator='1683' bot=False nick='Laureline - Plaisir (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=819170497132363799 name='Ereann cj vaux le penil' discriminator='2086' bot=False nick='Ereann - Vaux-le-Pénil (77)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=691588451547480076 name='Stéph_of28' discriminator='9983' bot=False nick='Stéphanie - Saint-Omer (62)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=812289741294534718 name='Noelly CJ de Chameyrat' discriminator='1221' bot=False nick='Noelly - Chameyrat (19)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=439791430651609089 name='Repti' discriminator='9965' bot=False nick='Enzo - Saint-Omer (62)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817369610051125309 name='Clémence' discriminator='9498' bot=False nick="Clémence - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=816646879135793152 name='titouan de poulainville' discriminator='6643' bot=False nick='Titouan - Poulainville (80)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=818559139415719976 name='KimieCJduGarric' discriminator='7403' bot=False nick='Kimie - Le Garric (81)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=816751853026017361 name='Lony cj poulainville' discriminator='5437' bot=False nick='Lony - Poulainville (80)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=653187728032399391 name='ImnotnathaYT' discriminator='8079' bot=False nick='Nathael - Bordeaux (33)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=821072189080076328 name='Marine du CJ de la Roche sur Yon' discriminator='0978' bot=False nick='Marine - La Roche-sur-Yon (85)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=752240686992064693 name='Meli melo' discriminator='9181' bot=False nick='Meryam - Forbach (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=683034848981680129 name="lily_blk CJ de yvré l'évêque" discriminator='7445' bot=False nick="Lily - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=766218397536354335 name='Abel_j' discriminator='2508' bot=False nick='Abel - Chamarande (91)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=689400323713794078 name='Marie-Agnès' discriminator='5423' bot=False nick='Marie-Agnès - Orgeval (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=811897434225377280 name='Héloïse CJ de Chameyrat' discriminator='5373' bot=False nick='Héloïse - Chameyrat (19)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=689473018740998159 name='Cathy' discriminator='7851' bot=False nick='Cathy - Sarreguemines (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=689815595746590832 name='jtmfort' discriminator='1427' bot=False nick='Lola - Vaux-le-Pénil (77)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=811893356618579978 name='Lily CJ de Rennes' discriminator='3212' bot=False nick='Lily - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=812625585276846130 name='YACINE CJ PLAISIR 78' discriminator='7816' bot=False nick='Yacine - Plaisir (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=822061661564174348 name='Nils05100' discriminator='4521' bot=False nick='Nils - Briançon (05)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=333364261688442890 name='Lucas ²' discriminator='1486' bot=False nick='Lucas - Forbach (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=811688103668219915 name='Lily CJ de Rennes' discriminator='0920' bot=False nick='Lily - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=812780108036571136 name='Chiara CJ de Niort' discriminator='8059' bot=False nick='Chiara - Niort (79)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=666896278021472287 name='Cassou-edn' discriminator='0209' bot=False nick="Cassandre - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=774024415859834911 name='malena' discriminator='8914' bot=False nick='Maléna - Cholet (49)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=694309330429804545 name='Valentine' discriminator='5125' bot=False nick='Valentine - Saint-Omer (62)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817867946701226003 name='paupau' discriminator='2647' bot=False nick='Pauline - Forbach (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=814861125580881940 name='Léane du CJ de Plaisir' discriminator='1982' bot=False nick='Léane - Plaisir (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=791638268247801898 name='Lucie - Forbach (57)' discriminator='7764' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=689063301199822971 name='Loane' discriminator='5676' bot=False nick='Loane - Chamarande (91)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=410138084181671938 name='Aiglor009' discriminator='3918' bot=False nick='Thomas - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=824269174246998076 name='Louna CJ de Luynes' discriminator='1106' bot=False nick='Louna - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=821332977371185152 name='catherine vitre' discriminator='6716' bot=False nick='Catherine - Vitré (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=811685909669216287 name='Lily CJ de Rennes' discriminator='7358' bot=False nick='Lily - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=826888582060179516 name='Laura CJ St Pierre du Mont' discriminator='3104' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=826007429703532545 name='Cassy CJ de Chamarande' discriminator='3125' bot=False nick='Cassy - Chamarande (91)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=772050348592201729 name='maelys CJ Pornic' discriminator='7949' bot=False nick='Maelys - Pornic (44)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=614958426849542157 name="Le P'tit Beurre Fou" discriminator='3503' bot=False nick='Eliott - Briançon (05)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=823644993427865690 name='Manonmr' discriminator='6723' bot=False nick='Manon - Le Garric (81)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=820014965867151370 name='erine du CJ de vaux le penil' discriminator='0120' bot=False nick='Erine - Vaux-le-Pénil (77)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=813532163655729172 name='Kelly CJ De Luynes' discriminator='4055' bot=False nick='Kelly - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=814843246046871604 name='Héléna CJ de Laon' discriminator='0749' bot=False nick='Héléna - Laon (02)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=723818066932269137 name='Marianne' discriminator='0263' bot=False nick='Marianne - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=814539477057011762 name='Clementine CJ de Millau' discriminator='9234' bot=False nick='Clementine - Millau (12)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=689831329331675143 name='Marywenn.Pornic(44)' discriminator='1346' bot=False nick='Maryween - Pornic (44)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=765294557252157440 name='Anaël CJ de Cluses' discriminator='7963' bot=False nick='Anaël - Cluses (74)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=796103288646926437 name='Garance' discriminator='7603' bot=False nick='Garance - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=690509463924506626 name='nightfox' discriminator='9964' bot=False nick='Esteban - Plaisir (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=819282970023559180 name='ines Cj thionville' discriminator='1353' bot=False nick='Inès - Thionville (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=814469566595596288 name='Lily CJ de Rennes' discriminator='3091' bot=False nick='Lily - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=811576583613579324 name='soizic du CJ de la roche sur yon' discriminator='8969' bot=False nick='Soizic - La Roche-sur-Yon (85)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=717309388830015528 name='Héloïse CJ de Pornic' discriminator='6617' bot=False nick='Héloise - Pornic (44)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=826007033266176011 name='Cassy CJ de Chamarande' discriminator='6404' bot=False nick='Cassy - Chamarande (91)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=825621468679110656 name='Lola du CJ du Garric' discriminator='6051' bot=False nick='Lola - Le Garric (81)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=793473737310601227 name='Alicia CJ de Menois' discriminator='4015' bot=False nick='Alicia - SPAT (10)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=429294921447637013 name='Cassie du CJ de Chamarande' discriminator='4125' bot=False nick='Cassie - Chamarande (91)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=812420593580244992 name='eliinaa_mrz' discriminator='0489' bot=False nick="Elina - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=791637538618998795 name='Tiâa-Forbach (57)' discriminator='2332' bot=False nick='Tiâa - Forbach (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=812365154184069132 name='Alma CJ de Bordeaux' discriminator='1871' bot=False nick='Alma - Bordeaux (33)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=821726042800390154 name='Valérie CJ Poulainville' discriminator='0191' bot=False nick='Valérie - Poulainville (80)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=554701108786888754 name='ness' discriminator='9391' bot=False nick="Ines - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=743880812981911563 name='lilie CJ Saint omer' discriminator='3660' bot=False nick='Lilie - Saint-Omer (62)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=688447791437054061 name='Manon Ricaud' discriminator='6573' bot=False nick='Manon - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=649282683255521305 name='Anaïs CJ de Saint Pierre du Mont' discriminator='1284' bot=False nick='Anaïs - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=811873653066301466 name='Margau CJ de Vaux-le-Pénil' discriminator='1974' bot=False nick='Margau - Vaux-le-Pénil (77)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=803322855290437703 name='Ewen du CJ de Chateaubourg' discriminator='7758' bot=False nick='Ewen - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=818553720135614496 name='Charlotte du CJ de le Garric' discriminator='9861' bot=False nick='Charlotte - Le Garric (81)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=811723077301174363 name='Marine CJ de Chateaubourg' discriminator='3546' bot=False nick='Marine - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=717010697120120862 name='Manon CJ orgeval' discriminator='5414' bot=False nick='Manon - Orgeval (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=783025428431634463 name='lilou' discriminator='0184' bot=False nick='Lilou - Saint-Omer (62)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=814843381876129834 name='Manon CJ de la Roche sur Yon' discriminator='0140' bot=False nick='Manon - La Roche-sur-Yon (85)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=812337799717584961 name='Luna CJ de Millau' discriminator='7128' bot=False nick='Luna - Millau (12)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817446940492562443 name='Aurore CJ Vaulx le Penil' discriminator='3737' bot=False nick='Aurore - Vaux-le-Pénil (77)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=824237075141230593 name='Chloé CJ Luynes' discriminator='7836' bot=False nick='Chloé - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=526740097698365440 name='Lgjump' discriminator='1054' bot=False nick='Thomas - Vaux-le-Pénil (77)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=812706223476178956 name='chachou' discriminator='7048' bot=False nick="Charlotte - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=814809886885937162 name='Lana du CJ de Chamarande' discriminator='4322' bot=False nick='Lana - Chamarande (91)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=812429809950785597 name='Sarah CJ de Chameyrat' discriminator='7571' bot=False nick='Sarah - Chameyrat (19)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=821766847556091944 name='Léandra cj de luynes' discriminator='3188' bot=False nick='Léandra - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=814554700983566356 name='Elsa CJ Lons Le Saunier' discriminator='3355' bot=False nick='Elsa - Lons-le-Saunier (39)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817456457397043241 name='Stephane (Thionville)' discriminator='1753' bot=False nick='Stéphane - Thionville (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=813424879491219456 name='Lily CJ de Rennes' discriminator='3661' bot=False nick='Lily - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=821799744996769822 name='Owen du CJ de luyne' discriminator='3245' bot=False nick='Owen - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=698528620423151706 name='Valentin CJ vaux-le-pénil' discriminator='8476' bot=False nick='Valentin - Vaux-le-Pénil (77)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=797583554988474418 name='Zoé- Forbach (57)' discriminator='7769' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=811574480299491338 name='Lorette CJ Saint Pierre du Mont' discriminator='1730' bot=False nick='Lorette - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=815284094417764383 name='Capucine CJ de Plaisir' discriminator='2186' bot=False nick='Capucine - Plaisir (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=573070802577129473 name="Romain CJ de Yvré l'Évèque" discriminator='9972' bot=False nick="Romain - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=812420035493625947 name="Mathéa.s de Yvré l'éveque 72" discriminator='3239' bot=False nick="Mathéa.s - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=688137172179615745 name='🌟 「 𝔹𝕒𝕓𝕪 𝕘𝕚𝕣𝕝 」 🌟' discriminator='7001' bot=False nick="Timothé - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=569597210728071210 name='Louve' discriminator='1683' bot=False nick='Laureline - Plaisir (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=819170497132363799 name='Ereann cj vaux le penil' discriminator='2086' bot=False nick='Ereann - Vaux-le-Pénil (77)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=691588451547480076 name='Stéph_of28' discriminator='9983' bot=False nick='Stéphanie - Saint-Omer (62)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=812289741294534718 name='Noelly CJ de Chameyrat' discriminator='1221' bot=False nick='Noelly - Chameyrat (19)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=439791430651609089 name='Repti' discriminator='9965' bot=False nick='Enzo - Saint-Omer (62)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817369610051125309 name='Clémence' discriminator='9498' bot=False nick="Clémence - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=816646879135793152 name='titouan de poulainville' discriminator='6643' bot=False nick='Titouan - Poulainville (80)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=818559139415719976 name='KimieCJduGarric' discriminator='7403' bot=False nick='Kimie - Le Garric (81)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=816751853026017361 name='Lony cj poulainville' discriminator='5437' bot=False nick='Lony - Poulainville (80)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=653187728032399391 name='ImnotnathaYT' discriminator='8079' bot=False nick='Nathael - Bordeaux (33)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=821072189080076328 name='Marine du CJ de la Roche sur Yon' discriminator='0978' bot=False nick='Marine - La Roche-sur-Yon (85)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=752240686992064693 name='Meli melo' discriminator='9181' bot=False nick='Meryam - Forbach (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=683034848981680129 name="lily_blk CJ de yvré l'évêque" discriminator='7445' bot=False nick="Lily - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=766218397536354335 name='Abel_j' discriminator='2508' bot=False nick='Abel - Chamarande (91)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=689400323713794078 name='Marie-Agnès' discriminator='5423' bot=False nick='Marie-Agnès - Orgeval (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=811897434225377280 name='Héloïse CJ de Chameyrat' discriminator='5373' bot=False nick='Héloïse - Chameyrat (19)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=689473018740998159 name='Cathy' discriminator='7851' bot=False nick='Cathy - Sarreguemines (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=689815595746590832 name='jtmfort' discriminator='1427' bot=False nick='Lola - Vaux-le-Pénil (77)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=811893356618579978 name='Lily CJ de Rennes' discriminator='3212' bot=False nick='Lily - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=812625585276846130 name='YACINE CJ PLAISIR 78' discriminator='7816' bot=False nick='Yacine - Plaisir (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=822061661564174348 name='Nils05100' discriminator='4521' bot=False nick='Nils - Briançon (05)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=333364261688442890 name='Lucas ²' discriminator='1486' bot=False nick='Lucas - Forbach (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=811688103668219915 name='Lily CJ de Rennes' discriminator='0920' bot=False nick='Lily - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=812780108036571136 name='Chiara CJ de Niort' discriminator='8059' bot=False nick='Chiara - Niort (79)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=666896278021472287 name='Cassou-edn' discriminator='0209' bot=False nick="Cassandre - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=774024415859834911 name='malena' discriminator='8914' bot=False nick='Maléna - Cholet (49)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=694309330429804545 name='Valentine' discriminator='5125' bot=False nick='Valentine - Saint-Omer (62)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817867946701226003 name='paupau' discriminator='2647' bot=False nick='Pauline - Forbach (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=814861125580881940 name='Léane du CJ de Plaisir' discriminator='1982' bot=False nick='Léane - Plaisir (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=771378220809453589 name='Dotmazy' discriminator='5284' bot=False nick='Thibault - Cj luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=791638268247801898 name='Lucie - Forbach (57)' discriminator='7764' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=689063301199822971 name='Loane' discriminator='5676' bot=False nick='Loane - Chamarande (91)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=410138084181671938 name='Aiglor009' discriminator='3918' bot=False nick='Thomas - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=824269174246998076 name='Louna CJ de Luynes' discriminator='1106' bot=False nick='Louna - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=821332977371185152 name='catherine vitre' discriminator='6716' bot=False nick='Catherine - Vitré (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=811685909669216287 name='Lily CJ de Rennes' discriminator='7358' bot=False nick='Lily - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=826888582060179516 name='Laura CJ St Pierre du Mont' discriminator='3104' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=826007429703532545 name='Cassy CJ de Chamarande' discriminator='3125' bot=False nick='Cassy - Chamarande (91)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=772050348592201729 name='maelys CJ Pornic' discriminator='7949' bot=False nick='Maelys - Pornic (44)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=614958426849542157 name="Le P'tit Beurre Fou" discriminator='3503' bot=False nick='Eliott - Briançon (05)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=823644993427865690 name='Manonmr' discriminator='6723' bot=False nick='Manon - Le Garric (81)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=820014965867151370 name='erine du CJ de vaux le penil' discriminator='0120' bot=False nick='Erine - Vaux-le-Pénil (77)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=813532163655729172 name='Kelly CJ De Luynes' discriminator='4055' bot=False nick='Kelly - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=814843246046871604 name='Héléna CJ de Laon' discriminator='0749' bot=False nick='Héléna - Laon (02)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=723818066932269137 name='Marianne' discriminator='0263' bot=False nick='Marianne - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=814539477057011762 name='Clementine CJ de Millau' discriminator='9234' bot=False nick='Clementine - Millau (12)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=689831329331675143 name='Marywenn.Pornic(44)' discriminator='1346' bot=False nick='Maryween - Pornic (44)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=765294557252157440 name='Anaël CJ de Cluses' discriminator='7963' bot=False nick='Anaël - Cluses (74)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=796103288646926437 name='Garance' discriminator='7603' bot=False nick='Garance - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=690509463924506626 name='nightfox' discriminator='9964' bot=False nick='Esteban - Plaisir (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=819282970023559180 name='ines Cj thionville' discriminator='1353' bot=False nick='Inès - Thionville (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=814469566595596288 name='Lily CJ de Rennes' discriminator='3091' bot=False nick='Lily - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=811576583613579324 name='soizic du CJ de la roche sur yon' discriminator='8969' bot=False nick='Soizic - La Roche-sur-Yon (85)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=717309388830015528 name='Héloïse CJ de Pornic' discriminator='6617' bot=False nick='Héloise - Pornic (44)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=826007033266176011 name='Cassy CJ de Chamarande' discriminator='6404' bot=False nick='Cassy - Chamarande (91)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=825621468679110656 name='Lola du CJ du Garric' discriminator='6051' bot=False nick='Lola - Le Garric (81)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=793473737310601227 name='Alicia CJ de Menois' discriminator='4015' bot=False nick='Alicia - SPAT (10)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=429294921447637013 name='Cassie du CJ de Chamarande' discriminator='4125' bot=False nick='Cassie - Chamarande (91)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=812420593580244992 name='eliinaa_mrz' discriminator='0489' bot=False nick="Elina - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=791637538618998795 name='Tiâa-Forbach (57)' discriminator='2332' bot=False nick='Tiâa - Forbach (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=812365154184069132 name='Alma CJ de Bordeaux' discriminator='1871' bot=False nick='Alma - Bordeaux (33)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=821726042800390154 name='Valérie CJ Poulainville' discriminator='0191' bot=False nick='Valérie - Poulainville (80)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=554701108786888754 name='ness' discriminator='9391' bot=False nick="Ines - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=743880812981911563 name='lilie CJ Saint omer' discriminator='3660' bot=False nick='Lilie - Saint-Omer (62)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=688447791437054061 name='Manon Ricaud' discriminator='6573' bot=False nick='Manon - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=649282683255521305 name='Anaïs CJ de Saint Pierre du Mont' discriminator='1284' bot=False nick='Anaïs - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=811873653066301466 name='Margau CJ de Vaux-le-Pénil' discriminator='1974' bot=False nick='Margau - Vaux-le-Pénil (77)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=803322855290437703 name='Ewen du CJ de Chateaubourg' discriminator='7758' bot=False nick='Ewen - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=818553720135614496 name='Charlotte du CJ de le Garric' discriminator='9861' bot=False nick='Charlotte - Le Garric (81)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=811723077301174363 name='Marine CJ de Chateaubourg' discriminator='3546' bot=False nick='Marine - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=717010697120120862 name='Manon CJ orgeval' discriminator='5414' bot=False nick='Manon - Orgeval (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=783025428431634463 name='lilou' discriminator='0184' bot=False nick='Lilou - Saint-Omer (62)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=814843381876129834 name='Manon CJ de la Roche sur Yon' discriminator='0140' bot=False nick='Manon - La Roche-sur-Yon (85)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=812337799717584961 name='Luna CJ de Millau' discriminator='7128' bot=False nick='Luna - Millau (12)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817446940492562443 name='Aurore CJ Vaulx le Penil' discriminator='3737' bot=False nick='Aurore - Vaux-le-Pénil (77)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=824237075141230593 name='Chloé CJ Luynes' discriminator='7836' bot=False nick='Chloé - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=526740097698365440 name='Lgjump' discriminator='1054' bot=False nick='Thomas - Vaux-le-Pénil (77)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=812706223476178956 name='chachou' discriminator='7048' bot=False nick="Charlotte - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=814809886885937162 name='Lana du CJ de Chamarande' discriminator='4322' bot=False nick='Lana - Chamarande (91)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=812429809950785597 name='Sarah CJ de Chameyrat' discriminator='7571' bot=False nick='Sarah - Chameyrat (19)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=821766847556091944 name='Léandra cj de luynes' discriminator='3188' bot=False nick='Léandra - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=814554700983566356 name='Elsa CJ Lons Le Saunier' discriminator='3355' bot=False nick='Elsa - Lons-le-Saunier (39)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817456457397043241 name='Stephane (Thionville)' discriminator='1753' bot=False nick='Stéphane - Thionville (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=813424879491219456 name='Lily CJ de Rennes' discriminator='3661' bot=False nick='Lily - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=821799744996769822 name='Owen du CJ de luyne' discriminator='3245' bot=False nick='Owen - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=698528620423151706 name='Valentin CJ vaux-le-pénil' discriminator='8476' bot=False nick='Valentin - Vaux-le-Pénil (77)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=797583554988474418 name='Zoé- Forbach (57)' discriminator='7769' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
@@ -3158,7 +3158,7 @@
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>[&lt;Member id=821843675272970272 name='Club jeunes Chamarande' discriminator='6857' bot=False nick='Léa - Chamarande (91)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=828949602937864202 name='Anne-Sophie - Forbach (57)' discriminator='7869' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=231129972755005440 name='Oyoelle' discriminator='7903' bot=False nick='Elwenn - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=828320232971829299 name='julie37' discriminator='9767' bot=False nick='Julie - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=826134409349955594 name='Mary-Chateaubourg35' discriminator='3382' bot=False nick='Mary - Chateaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=812399451427307542 name='sarah kervinio Yvré' discriminator='5630' bot=False nick="Sarah - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817494596170416128 name='Dragana' discriminator='8632' bot=False nick='Dragana - Laon (02)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817462125815398411 name='Cécile Encadrante CJ Luynes (37)' discriminator='4741' bot=False nick='Cécile - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=689875189814657053 name='Hélène - Encadrante SPA - Millau' discriminator='0248' bot=False nick='Hélène - Millau (12)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=812023228167618601 name='Sylvie CJ St OMER' discriminator='3410' bot=False nick='Sylvie - Saint-Omer (62)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817630483294060595 name='Catherine Fuseau' discriminator='8144' bot=False nick='Catherine - SPAT (10)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=725471539365150867 name='Erwan' discriminator='0084' bot=False nick='Erwan - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817456802983575553 name='Alix CJ SPDM' discriminator='4012' bot=False nick='Alix - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817472074028941322 name='Marinette CJ de Luynes' discriminator='4290' bot=False nick='Marinette - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=713390694806323312 name='Justine' discriminator='8951' bot=False nick='Justine - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817494454927491093 name='Maria CJ La Roche sur Yon' discriminator='7686' bot=False nick='Maria - La Roche-sur-Yon (85)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=818083516234989588 name='Chantale CJ de Plaisir' discriminator='3278' bot=False nick='Chantale - Plaisir (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817531532180717639 name='Hervé Pierrick' discriminator='9042' bot=False nick="Pierrick - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=818876857675677741 name='Anne sophie Cluses' discriminator='2450' bot=False nick='Anne - Cluses (74)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=806174108286451764 name='Reale COUCHAUX' discriminator='6300' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=824916103918387223 name='Patou' discriminator='8474' bot=False nick='Patou - Pornic (44)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=819231783635648543 name='imogen CJ de briancon' discriminator='1398' bot=False nick='Imogen - Briançon (05)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=818072289346191395 name='Trinity49' discriminator='5916' bot=False nick='Didier - Cholet (49)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=811656729812664370 name='Hugo CJ Saint Pierre du Mont' discriminator='2618' bot=False nick='Céline - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817468032645070909 name='MariaF' discriminator='9993' bot=False nick='Maria - La Roche-sur-Yon (85)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=387907535019048961 name='Pauline' discriminator='8887' bot=False nick='Pauline - Chateaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=779255638911221790 name='Clémentine CJ SaintPierreDuMont' discriminator='3516' bot=False nick='Clémentine - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=809826133755428886 name='Ragnarock' discriminator='1491' bot=False nick='Élodie - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817668024613339177 name='Audrey (endadrante 81)' discriminator='4921' bot=False nick='Audrey - Le Garric (81)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817502019048439889 name='Virginie' discriminator='0867' bot=False nick='Virginie - Arry (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=294200564357791745 name='Cédric' discriminator='6625' bot=False nick='Cédric - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=818560915817103370 name='caroline enc.CJ Thionville' discriminator='5118' bot=False nick='Caroline - Thionville (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=739521549132103712 name='sgodefroy' discriminator='7405' bot=False nick='Stephane - Thionville (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817455331637461033 name='Romane Chateaubourg' discriminator='6316' bot=False nick='Romane - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=821843675272970272 name='Club jeunes Chamarande' discriminator='6857' bot=False nick='Léa - Chamarande (91)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=828949602937864202 name='Anne-Sophie - Forbach (57)' discriminator='7869' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=231129972755005440 name='Oyoelle' discriminator='7903' bot=False nick='Elwenn - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=828320232971829299 name='julie37' discriminator='9767' bot=False nick='Julie - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=826134409349955594 name='Mary-Chateaubourg35' discriminator='3382' bot=False nick='Mary - Chateaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=812399451427307542 name='sarah kervinio Yvré' discriminator='5630' bot=False nick="Sarah - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817494596170416128 name='Dragana' discriminator='8632' bot=False nick='Dragana - Laon (02)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817462125815398411 name='Cécile Encadrante CJ Luynes (37)' discriminator='4741' bot=False nick='Cécile - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=689875189814657053 name='Hélène - Encadrante SPA - Millau' discriminator='0248' bot=False nick='Hélène - Millau (12)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=812023228167618601 name='Sylvie CJ St OMER' discriminator='3410' bot=False nick='Sylvie - Saint-Omer (62)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817630483294060595 name='Catherine Fuseau' discriminator='8144' bot=False nick='Catherine - SPAT (10)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=725471539365150867 name='Erwan' discriminator='0084' bot=False nick='Erwan - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817456802983575553 name='Alix CJ SPDM' discriminator='4012' bot=False nick='Alix - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817472074028941322 name='Marinette CJ de Luynes' discriminator='4290' bot=False nick='Marinette - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=713390694806323312 name='Justine' discriminator='8951' bot=False nick='Justine - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817494454927491093 name='Maria CJ La Roche sur Yon' discriminator='7686' bot=False nick='Maria - La Roche-sur-Yon (85)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=818083516234989588 name='Chantale CJ de Plaisir' discriminator='3278' bot=False nick='Chantale - Plaisir (78)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817531532180717639 name='Hervé Pierrick' discriminator='9042' bot=False nick="Pierrick - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=818876857675677741 name='Anne sophie Cluses' discriminator='2450' bot=False nick='Anne - Cluses (74)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=806174108286451764 name='Reale COUCHAUX' discriminator='6300' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=824916103918387223 name='Patou' discriminator='8474' bot=False nick='Patou - Pornic (44)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=819231783635648543 name='imogen CJ de briancon' discriminator='1398' bot=False nick='Imogen - Briançon (05)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=818072289346191395 name='Trinity49' discriminator='5916' bot=False nick='Didier - Cholet (49)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=811656729812664370 name='Hugo CJ Saint Pierre du Mont' discriminator='2618' bot=False nick='Céline - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817468032645070909 name='MariaF' discriminator='9993' bot=False nick='Maria - La Roche-sur-Yon (85)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=387907535019048961 name='Pauline' discriminator='8887' bot=False nick='Pauline - Chateaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=779255638911221790 name='Clémentine CJ SaintPierreDuMont' discriminator='3516' bot=False nick='Clémentine - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=809826133755428886 name='Ragnarock' discriminator='1491' bot=False nick='Élodie - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817668024613339177 name='Audrey (endadrante 81)' discriminator='4921' bot=False nick='Audrey - Le Garric (81)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817502019048439889 name='Virginie' discriminator='0867' bot=False nick='Virginie - Arry (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=294200564357791745 name='Cédric' discriminator='6625' bot=False nick='Cédric - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=818560915817103370 name='caroline enc.CJ Thionville' discriminator='5118' bot=False nick='Caroline - Thionville (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=739521549132103712 name='sgodefroy' discriminator='7405' bot=False nick='Stephane - Thionville (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817455331637461033 name='Romane Chateaubourg' discriminator='6316' bot=False nick='Romane - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
@@ -3217,7 +3217,7 @@
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>[&lt;Member id=812399451427307542 name='sarah kervinio Yvré' discriminator='5630' bot=False nick="Sarah - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817630483294060595 name='Catherine Fuseau' discriminator='8144' bot=False nick='Catherine - SPAT (10)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817472074028941322 name='Marinette CJ de Luynes' discriminator='4290' bot=False nick='Marinette - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817494454927491093 name='Maria CJ La Roche sur Yon' discriminator='7686' bot=False nick='Maria - La Roche-sur-Yon (85)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=818876857675677741 name='Anne sophie Cluses' discriminator='2450' bot=False nick='Anne - Cluses (74)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=824916103918387223 name='Patou' discriminator='8474' bot=False nick='Patou - Pornic (44)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=819231783635648543 name='imogen CJ de briancon' discriminator='1398' bot=False nick='Imogen - Briançon (05)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=811656729812664370 name='Hugo CJ Saint Pierre du Mont' discriminator='2618' bot=False nick='Céline - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817468032645070909 name='MariaF' discriminator='9993' bot=False nick='Maria - La Roche-sur-Yon (85)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817668024613339177 name='Audrey (endadrante 81)' discriminator='4921' bot=False nick='Audrey - Le Garric (81)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817502019048439889 name='Virginie' discriminator='0867' bot=False nick='Virginie - Arry (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=294200564357791745 name='Cédric' discriminator='6625' bot=False nick='Cédric - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=739521549132103712 name='sgodefroy' discriminator='7405' bot=False nick='Stephane - Thionville (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=817455331637461033 name='Romane Chateaubourg' discriminator='6316' bot=False nick='Romane - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=812399451427307542 name='sarah kervinio Yvré' discriminator='5630' bot=False nick="Sarah - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817630483294060595 name='Catherine Fuseau' discriminator='8144' bot=False nick='Catherine - SPAT (10)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817472074028941322 name='Marinette CJ de Luynes' discriminator='4290' bot=False nick='Marinette - Luynes (37)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817494454927491093 name='Maria CJ La Roche sur Yon' discriminator='7686' bot=False nick='Maria - La Roche-sur-Yon (85)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=818876857675677741 name='Anne sophie Cluses' discriminator='2450' bot=False nick='Anne - Cluses (74)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=824916103918387223 name='Patou' discriminator='8474' bot=False nick='Patou - Pornic (44)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=819231783635648543 name='imogen CJ de briancon' discriminator='1398' bot=False nick='Imogen - Briançon (05)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=811656729812664370 name='Hugo CJ Saint Pierre du Mont' discriminator='2618' bot=False nick='Céline - SPDM (40)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817468032645070909 name='MariaF' discriminator='9993' bot=False nick='Maria - La Roche-sur-Yon (85)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817668024613339177 name='Audrey (endadrante 81)' discriminator='4921' bot=False nick='Audrey - Le Garric (81)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817502019048439889 name='Virginie' discriminator='0867' bot=False nick='Virginie - Arry (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=294200564357791745 name='Cédric' discriminator='6625' bot=False nick='Cédric - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=739521549132103712 name='sgodefroy' discriminator='7405' bot=False nick='Stephane - Thionville (57)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=817455331637461033 name='Romane Chateaubourg' discriminator='6316' bot=False nick='Romane - Châteaubourg (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
@@ -3276,7 +3276,7 @@
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>[&lt;Member id=812399451427307542 name='sarah kervinio Yvré' discriminator='5630' bot=False nick="Sarah - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=812399451427307542 name='sarah kervinio Yvré' discriminator='5630' bot=False nick="Sarah - Yvré l'Évêque (72)" guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
@@ -3335,7 +3335,7 @@
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>[&lt;Member id=817684166274842654 name='Jean DUQUESNOIS' discriminator='2933' bot=False nick='Jean - Vallérargues (30)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=817684166274842654 name='Jean DUQUESNOIS' discriminator='2933' bot=False nick='Jean - Vallérargues (30)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
@@ -3394,7 +3394,7 @@
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>[&lt;Member id=674885857458651161 name='MemberList' discriminator='4997' bot=True nick='🐶Hachikō' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=324631108731928587 name='Simple Poll' discriminator='9879' bot=True nick='🐶Laïka' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=159985870458322944 name='MEE6' discriminator='4876' bot=True nick='🐱Simon' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=558996910581612545 name='QuizBot' discriminator='0134' bot=True nick='🐶Togo' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=294200564357791745 name='Cédric' discriminator='6625' bot=False nick='Cédric - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=818564026237452350 name='Ohana' discriminator='1949' bot=True nick='🐶 Ohana' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=674885857458651161 name='MemberList' discriminator='4997' bot=True nick='🐶Hachikō' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=324631108731928587 name='Simple Poll' discriminator='9879' bot=True nick='🐶Laïka' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=159985870458322944 name='MEE6' discriminator='4876' bot=True nick='🐱Simon' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=558996910581612545 name='QuizBot' discriminator='0134' bot=True nick='🐶Togo' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=294200564357791745 name='Cédric' discriminator='6625' bot=False nick='Cédric - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=818564026237452350 name='Ohana' discriminator='1949' bot=True nick='🐶 Ohana' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
@@ -3453,7 +3453,7 @@
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>[&lt;Member id=806174253849378839 name='Kévin DOUANGSAVATH' discriminator='6501' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=806134269557604373 name='Société Protectrice des Animaux' discriminator='3238' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=806174108286451764 name='Reale COUCHAUX' discriminator='6300' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;, &lt;Member id=294200564357791745 name='Cédric' discriminator='6625' bot=False nick='Cédric - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=150&gt;&gt;]</t>
+          <t>[&lt;Member id=806174253849378839 name='Kévin DOUANGSAVATH' discriminator='6501' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=806134269557604373 name='Société Protectrice des Animaux' discriminator='3238' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=806174108286451764 name='Reale COUCHAUX' discriminator='6300' bot=False nick=None guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;, &lt;Member id=294200564357791745 name='Cédric' discriminator='6625' bot=False nick='Cédric - Rennes (35)' guild=&lt;Guild id=806137569116291102 name='Clubs Jeunes SPA' shard_id=None chunked=True member_count=151&gt;&gt;]</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">

</xml_diff>